<commit_message>
Small correction in US04 and copy of sprint B to continue development
</commit_message>
<xml_diff>
--- a/PI-2023-24 Self-Assessment.xlsx
+++ b/PI-2023-24 Self-Assessment.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dinia\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\aplicacoes\JetBrain\InteliJ_Projects\lei-24-s2-1do-g164v2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8254AF0F-8B38-44DF-B7A2-958CF14FA4F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3509224F-D647-444D-9F99-FFD375440204}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Group and Self Assessment" sheetId="2" r:id="rId1"/>
@@ -1767,8 +1767,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:T36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="V10" sqref="V10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2467,8 +2467,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView topLeftCell="A4" zoomScale="72" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2573,7 +2573,7 @@
         <v>1230776</v>
       </c>
       <c r="C6" s="29">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D6" s="60"/>
       <c r="E6" s="31" t="s">
@@ -2693,7 +2693,7 @@
         <v>1230609</v>
       </c>
       <c r="C10" s="29">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D10" s="60"/>
       <c r="E10" s="14" t="s">
@@ -3135,7 +3135,7 @@
   <dimension ref="A1:Z10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3284,13 +3284,13 @@
         <v>0.1</v>
       </c>
       <c r="C4" s="25">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D4" s="25">
         <v>4</v>
       </c>
       <c r="E4" s="25">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F4" s="25">
         <v>4</v>
@@ -3308,7 +3308,7 @@
       <c r="Q4" s="25"/>
       <c r="R4" s="27">
         <f t="shared" ref="R4:R7" si="0">AVERAGE(C4:Q4)</f>
-        <v>4</v>
+        <v>4.5</v>
       </c>
       <c r="S4" s="7" t="s">
         <v>52</v>
@@ -3339,13 +3339,13 @@
         <v>0.2</v>
       </c>
       <c r="C5" s="25">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D5" s="25">
         <v>5</v>
       </c>
       <c r="E5" s="25">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F5" s="25">
         <v>5</v>
@@ -3363,7 +3363,7 @@
       <c r="Q5" s="25"/>
       <c r="R5" s="27">
         <f t="shared" si="0"/>
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="S5" s="7" t="s">
         <v>59</v>
@@ -3498,7 +3498,7 @@
       </c>
       <c r="C8" s="7">
         <f t="shared" ref="C8:Q8" si="1">SUMPRODUCT(C4:C7,$B$4:$B$7)</f>
-        <v>3.2</v>
+        <v>3.5</v>
       </c>
       <c r="D8" s="7">
         <f t="shared" si="1"/>
@@ -3506,7 +3506,7 @@
       </c>
       <c r="E8" s="7">
         <f t="shared" si="1"/>
-        <v>3.2</v>
+        <v>3.5</v>
       </c>
       <c r="F8" s="7">
         <f t="shared" si="1"/>
@@ -3573,7 +3573,7 @@
       <c r="B9" s="23"/>
       <c r="C9" s="23">
         <f>C8/5*20</f>
-        <v>12.8</v>
+        <v>14</v>
       </c>
       <c r="D9" s="23">
         <f t="shared" ref="D9:Q9" si="2">D8/5*20</f>
@@ -3581,7 +3581,7 @@
       </c>
       <c r="E9" s="23">
         <f t="shared" si="2"/>
-        <v>12.8</v>
+        <v>14</v>
       </c>
       <c r="F9" s="23">
         <f t="shared" si="2"/>
@@ -3660,8 +3660,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:Z17"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3978,10 +3978,10 @@
         <v>4</v>
       </c>
       <c r="E7" s="25">
+        <v>5</v>
+      </c>
+      <c r="F7" s="25">
         <v>4</v>
-      </c>
-      <c r="F7" s="25">
-        <v>3</v>
       </c>
       <c r="G7" s="25"/>
       <c r="H7" s="25"/>
@@ -3996,7 +3996,7 @@
       <c r="Q7" s="25"/>
       <c r="R7" s="55">
         <f t="shared" si="0"/>
-        <v>3.75</v>
+        <v>4.25</v>
       </c>
       <c r="S7" s="59" t="s">
         <v>94</v>
@@ -4027,16 +4027,16 @@
         <v>0.1</v>
       </c>
       <c r="C8" s="25">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D8" s="25">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E8" s="25">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F8" s="25">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G8" s="25"/>
       <c r="H8" s="25"/>
@@ -4051,7 +4051,7 @@
       <c r="Q8" s="25"/>
       <c r="R8" s="55">
         <f t="shared" ref="R8:R12" si="1">AVERAGE(C8:Q8)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="S8" s="59" t="s">
         <v>94</v>
@@ -4402,19 +4402,19 @@
       </c>
       <c r="C15" s="7">
         <f>SUMPRODUCT(C4:C14,$B$4:$B$14)</f>
-        <v>3.5500000000000003</v>
+        <v>3.7500000000000004</v>
       </c>
       <c r="D15" s="7">
         <f t="shared" ref="D15:Q15" si="4">SUMPRODUCT(D4:D14,$B$4:$B$14)</f>
-        <v>3.8</v>
+        <v>4</v>
       </c>
       <c r="E15" s="7">
         <f t="shared" si="4"/>
-        <v>3.7</v>
+        <v>3.95</v>
       </c>
       <c r="F15" s="7">
         <f t="shared" si="4"/>
-        <v>3.8</v>
+        <v>4.05</v>
       </c>
       <c r="G15" s="7">
         <f t="shared" si="4"/>
@@ -4477,19 +4477,19 @@
       <c r="B16" s="23"/>
       <c r="C16" s="23">
         <f>C15/5*20</f>
-        <v>14.200000000000001</v>
+        <v>15.000000000000002</v>
       </c>
       <c r="D16" s="23">
         <f t="shared" ref="D16:Q16" si="5">D15/5*20</f>
-        <v>15.2</v>
+        <v>16</v>
       </c>
       <c r="E16" s="23">
         <f t="shared" si="5"/>
-        <v>14.8</v>
+        <v>15.8</v>
       </c>
       <c r="F16" s="23">
         <f t="shared" si="5"/>
-        <v>15.2</v>
+        <v>16.2</v>
       </c>
       <c r="G16" s="23">
         <f t="shared" si="5"/>
@@ -4560,6 +4560,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005836243B3C47804EAF5FFDD9F066FCC7" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9d21ddf3f0b128e39c9d770c8c903166">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a1e3ca88-8ae5-4fd0-ba37-40ce669fcbb0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b0326308c339679ad994635f2c691325" ns2:_="">
     <xsd:import namespace="a1e3ca88-8ae5-4fd0-ba37-40ce669fcbb0"/>
@@ -4743,7 +4749,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -4752,13 +4758,23 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D8D82CB-2E6F-4A14-B6B4-DFDD1BBD70FC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="a1e3ca88-8ae5-4fd0-ba37-40ce669fcbb0"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23B77F7C-EE47-4FBD-B078-6536C1487A1E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4776,26 +4792,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F61419B8-A98A-41CD-95EE-48A4F975B8D1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D8D82CB-2E6F-4A14-B6B4-DFDD1BBD70FC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="a1e3ca88-8ae5-4fd0-ba37-40ce669fcbb0"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>